<commit_message>
fix issue carga masiva de aclendario
</commit_message>
<xml_diff>
--- a/src/assets/files/15.CalendarioAnual.xlsx
+++ b/src/assets/files/15.CalendarioAnual.xlsx
@@ -1,19 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\avictoria\Documents\Proyectos\AgendaDigital\ARCHIVOS PRUEBA\oficiales\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{75B177DF-0262-482C-9876-D06D811FD845}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61943AF0-953C-4662-8A3F-44FA083CA7D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" activeTab="2" xr2:uid="{76E7FC68-D242-465E-8EB4-3CC40106161F}"/>
+    <workbookView xWindow="-16560" yWindow="-3274" windowWidth="16663" windowHeight="9017" activeTab="2" xr2:uid="{76E7FC68-D242-465E-8EB4-3CC40106161F}"/>
   </bookViews>
   <sheets>
-    <sheet name="A_servicios_especialidades" sheetId="1" r:id="rId1"/>
+    <sheet name="E_14_GRUPOS_Programas" sheetId="1" r:id="rId1"/>
     <sheet name="B_4_UBICACIONES" sheetId="2" r:id="rId2"/>
     <sheet name="F_CalendarioAnual" sheetId="3" r:id="rId3"/>
   </sheets>
@@ -37,46 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="34">
-  <si>
-    <t>CLAVE ESPECIALIDAD</t>
-  </si>
-  <si>
-    <t>DESCRIPCIÓN ESPECIALIDAD</t>
-  </si>
-  <si>
-    <t>IND_CE</t>
-  </si>
-  <si>
-    <t>IND_HOSP</t>
-  </si>
-  <si>
-    <t>IND_IQ</t>
-  </si>
-  <si>
-    <t>IND_NIVEL1</t>
-  </si>
-  <si>
-    <t>IND_NIVEL2</t>
-  </si>
-  <si>
-    <t>IND_NIVEL3</t>
-  </si>
-  <si>
-    <t>IND_CSS</t>
-  </si>
-  <si>
-    <t>FEC_BAJA</t>
-  </si>
-  <si>
-    <t>FEC_ALTA</t>
-  </si>
-  <si>
-    <t>FEC_ACTUALIZACION</t>
-  </si>
-  <si>
-    <t>AC01</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="76">
   <si>
     <t xml:space="preserve">Atención Médica Continúa </t>
   </si>
@@ -108,9 +69,6 @@
     <t>Trab_Social_01</t>
   </si>
   <si>
-    <t>SERVICIOS / ESPECIALIDADES</t>
-  </si>
-  <si>
     <t>UBICACIÓN</t>
   </si>
   <si>
@@ -132,13 +90,181 @@
     <t>MAXIMO DE PARTICIPANTES</t>
   </si>
   <si>
-    <t>Adulto Mayores</t>
-  </si>
-  <si>
     <t>Consultorio</t>
   </si>
   <si>
     <t>UMF12</t>
+  </si>
+  <si>
+    <t>PROGRAMA</t>
+  </si>
+  <si>
+    <t>VIH</t>
+  </si>
+  <si>
+    <t>DESCRIPCION GRUPO / PROGRAMA</t>
+  </si>
+  <si>
+    <t>CODIGO</t>
+  </si>
+  <si>
+    <t>DESCRIPCION ACTIVIDAD</t>
+  </si>
+  <si>
+    <t>Tour  Quirúrgico</t>
+  </si>
+  <si>
+    <t>TS2.C</t>
+  </si>
+  <si>
+    <t>Tour Quirúrgico</t>
+  </si>
+  <si>
+    <t>Trabajo Social</t>
+  </si>
+  <si>
+    <t>Tour Obstétrico</t>
+  </si>
+  <si>
+    <t>TS2.B</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Tour Quimioterapia</t>
+  </si>
+  <si>
+    <t>Z71.8</t>
+  </si>
+  <si>
+    <t>Necesidad de información sobre cáncer</t>
+  </si>
+  <si>
+    <t>Donación de  Sangre.</t>
+  </si>
+  <si>
+    <t>TS1.O</t>
+  </si>
+  <si>
+    <t>Necesidad de información para donación de sangre</t>
+  </si>
+  <si>
+    <t>TS1.T</t>
+  </si>
+  <si>
+    <t>Paciente integrado a programa de VIH/SIDA</t>
+  </si>
+  <si>
+    <t>Diálisis</t>
+  </si>
+  <si>
+    <t>TS1.W</t>
+  </si>
+  <si>
+    <t>Paciente integrado a programa de Diálisis</t>
+  </si>
+  <si>
+    <t>Hemodiálisis</t>
+  </si>
+  <si>
+    <t>TS1.U</t>
+  </si>
+  <si>
+    <t>Paciente integrado a programa de Hemodiálisis</t>
+  </si>
+  <si>
+    <t>CACU</t>
+  </si>
+  <si>
+    <t>CAMA</t>
+  </si>
+  <si>
+    <t>TS1.X</t>
+  </si>
+  <si>
+    <t>Paciente integrado a clínica de mama</t>
+  </si>
+  <si>
+    <t>GeriatrIMSS</t>
+  </si>
+  <si>
+    <t>TS1</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>Lactancia Materna</t>
+  </si>
+  <si>
+    <t>TS1.S</t>
+  </si>
+  <si>
+    <t>Necesidad de información para la lactancia materna</t>
+  </si>
+  <si>
+    <t>Cuidados del paciente post trasplante</t>
+  </si>
+  <si>
+    <t>TS1.N</t>
+  </si>
+  <si>
+    <t>Necesidad de información para donación de órganos y tejidos</t>
+  </si>
+  <si>
+    <t>Educación para pacientes prematuros</t>
+  </si>
+  <si>
+    <t>TS1.L</t>
+  </si>
+  <si>
+    <t>Expectativas diferentes de los integrantes de la familia que inciden en salud</t>
+  </si>
+  <si>
+    <t>Cuidados de pacientes oncológicos</t>
+  </si>
+  <si>
+    <t>Autocuidado de la Salud</t>
+  </si>
+  <si>
+    <t>Cuidados post cateterismo cardiaco</t>
+  </si>
+  <si>
+    <t>Ts2</t>
+  </si>
+  <si>
+    <t>Yoga prenatal</t>
+  </si>
+  <si>
+    <t>Grupos voluntarios</t>
+  </si>
+  <si>
+    <t>TS2.H</t>
+  </si>
+  <si>
+    <t>Incorporación a grupos de autoayuda</t>
+  </si>
+  <si>
+    <t>Otros</t>
+  </si>
+  <si>
+    <t>TS3</t>
+  </si>
+  <si>
+    <t>ADEC</t>
+  </si>
+  <si>
+    <t>TS1.V</t>
+  </si>
+  <si>
+    <t>Paciente integrado al programa de DEC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Planificación Familiar </t>
+  </si>
+  <si>
+    <t>Z30.0</t>
+  </si>
+  <si>
+    <t>Necesidad de información en Planificación Familiar</t>
   </si>
 </sst>
 </file>
@@ -499,104 +625,346 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{64CCAEAA-4231-4770-9010-191EE5FD3295}">
-  <dimension ref="A1:L191"/>
+  <dimension ref="A1:J191"/>
   <sheetViews>
     <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="I17" sqref="I17"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="23.33203125" customWidth="1"/>
+    <col min="1" max="1" width="23.33203125" customWidth="1"/>
+    <col min="4" max="4" width="21.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>21</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
+        <v>22</v>
       </c>
       <c r="C1" t="s">
-        <v>2</v>
+        <v>23</v>
       </c>
       <c r="D1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" t="s">
-        <v>9</v>
-      </c>
-      <c r="K1" t="s">
-        <v>10</v>
-      </c>
-      <c r="L1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="B2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C2">
-        <v>1</v>
-      </c>
-      <c r="D2">
-        <v>0</v>
-      </c>
-      <c r="E2">
-        <v>0</v>
-      </c>
-      <c r="F2">
-        <v>1</v>
-      </c>
-      <c r="G2">
-        <v>1</v>
-      </c>
-      <c r="H2">
-        <v>1</v>
-      </c>
-      <c r="I2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="10:10" x14ac:dyDescent="0.3">
-      <c r="J26" s="1"/>
-    </row>
-    <row r="42" spans="10:10" x14ac:dyDescent="0.3">
-      <c r="J42" s="1"/>
-    </row>
-    <row r="43" spans="10:10" x14ac:dyDescent="0.3">
-      <c r="J43" s="1"/>
-    </row>
-    <row r="52" spans="10:10" x14ac:dyDescent="0.3">
-      <c r="J52" s="1"/>
-    </row>
-    <row r="65" spans="10:10" x14ac:dyDescent="0.3">
-      <c r="J65" s="1"/>
-    </row>
-    <row r="190" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K190" s="1"/>
-    </row>
-    <row r="191" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K191" s="1"/>
+        <v>25</v>
+      </c>
+      <c r="C2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>28</v>
+      </c>
+      <c r="B3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C3" t="s">
+        <v>28</v>
+      </c>
+      <c r="D3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>30</v>
+      </c>
+      <c r="B4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C4" t="s">
+        <v>32</v>
+      </c>
+      <c r="D4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>33</v>
+      </c>
+      <c r="B5" t="s">
+        <v>34</v>
+      </c>
+      <c r="C5" t="s">
+        <v>35</v>
+      </c>
+      <c r="D5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>20</v>
+      </c>
+      <c r="B6" t="s">
+        <v>36</v>
+      </c>
+      <c r="C6" t="s">
+        <v>37</v>
+      </c>
+      <c r="D6" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>38</v>
+      </c>
+      <c r="B7" t="s">
+        <v>39</v>
+      </c>
+      <c r="C7" t="s">
+        <v>40</v>
+      </c>
+      <c r="D7" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>41</v>
+      </c>
+      <c r="B8" t="s">
+        <v>42</v>
+      </c>
+      <c r="C8" t="s">
+        <v>43</v>
+      </c>
+      <c r="D8" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>44</v>
+      </c>
+      <c r="B9" t="s">
+        <v>31</v>
+      </c>
+      <c r="C9" t="s">
+        <v>32</v>
+      </c>
+      <c r="D9" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>45</v>
+      </c>
+      <c r="B10" t="s">
+        <v>46</v>
+      </c>
+      <c r="C10" t="s">
+        <v>47</v>
+      </c>
+      <c r="D10" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>48</v>
+      </c>
+      <c r="B11" t="s">
+        <v>49</v>
+      </c>
+      <c r="C11" t="s">
+        <v>50</v>
+      </c>
+      <c r="D11" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>51</v>
+      </c>
+      <c r="B12" t="s">
+        <v>52</v>
+      </c>
+      <c r="C12" t="s">
+        <v>53</v>
+      </c>
+      <c r="D12" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>54</v>
+      </c>
+      <c r="B13" t="s">
+        <v>55</v>
+      </c>
+      <c r="C13" t="s">
+        <v>56</v>
+      </c>
+      <c r="D13" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>57</v>
+      </c>
+      <c r="B14" t="s">
+        <v>58</v>
+      </c>
+      <c r="C14" t="s">
+        <v>59</v>
+      </c>
+      <c r="D14" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>60</v>
+      </c>
+      <c r="B15" t="s">
+        <v>31</v>
+      </c>
+      <c r="C15" t="s">
+        <v>32</v>
+      </c>
+      <c r="D15" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>61</v>
+      </c>
+      <c r="B16" t="s">
+        <v>58</v>
+      </c>
+      <c r="C16" t="s">
+        <v>59</v>
+      </c>
+      <c r="D16" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>62</v>
+      </c>
+      <c r="B17" t="s">
+        <v>63</v>
+      </c>
+      <c r="C17" t="s">
+        <v>50</v>
+      </c>
+      <c r="D17" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>64</v>
+      </c>
+      <c r="B18" t="s">
+        <v>58</v>
+      </c>
+      <c r="C18" t="s">
+        <v>59</v>
+      </c>
+      <c r="D18" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>65</v>
+      </c>
+      <c r="B19" t="s">
+        <v>66</v>
+      </c>
+      <c r="C19" t="s">
+        <v>67</v>
+      </c>
+      <c r="D19" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>68</v>
+      </c>
+      <c r="B20" t="s">
+        <v>69</v>
+      </c>
+      <c r="C20" t="s">
+        <v>50</v>
+      </c>
+      <c r="D20" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>70</v>
+      </c>
+      <c r="B21" t="s">
+        <v>71</v>
+      </c>
+      <c r="C21" t="s">
+        <v>72</v>
+      </c>
+      <c r="D21" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>73</v>
+      </c>
+      <c r="B22" t="s">
+        <v>74</v>
+      </c>
+      <c r="C22" t="s">
+        <v>75</v>
+      </c>
+      <c r="D22" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="I26" s="1"/>
+    </row>
+    <row r="42" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I42" s="1"/>
+    </row>
+    <row r="43" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I43" s="1"/>
+    </row>
+    <row r="52" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I52" s="1"/>
+    </row>
+    <row r="65" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I65" s="1"/>
+    </row>
+    <row r="190" spans="10:10" x14ac:dyDescent="0.3">
+      <c r="J190" s="1"/>
+    </row>
+    <row r="191" spans="10:10" x14ac:dyDescent="0.3">
+      <c r="J191" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -624,25 +992,25 @@
   <sheetData>
     <row r="1" spans="1:7" s="2" customFormat="1" ht="28.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
-        <v>14</v>
+        <v>1</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>15</v>
+        <v>2</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>16</v>
+        <v>3</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>17</v>
+        <v>4</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>18</v>
+        <v>5</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>20</v>
+        <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
@@ -650,19 +1018,19 @@
         <v>6</v>
       </c>
       <c r="B2" t="s">
-        <v>21</v>
+        <v>8</v>
       </c>
       <c r="C2" t="s">
-        <v>22</v>
+        <v>9</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>32</v>
+        <v>17</v>
       </c>
       <c r="F2" t="s">
-        <v>13</v>
+        <v>0</v>
       </c>
       <c r="G2" t="s">
-        <v>33</v>
+        <v>18</v>
       </c>
     </row>
   </sheetData>
@@ -672,13 +1040,13 @@
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{5262BBD6-F35A-4EFA-8784-122DD4E3CC3F}">
           <x14:formula1>
-            <xm:f>A_servicios_especialidades!$B$2:$B$27</xm:f>
+            <xm:f>E_14_GRUPOS_Programas!$A$2:$A$27</xm:f>
           </x14:formula1>
           <xm:sqref>F29:F97</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{D7CD36EE-C343-4AF1-AFC1-30B4B1AC8850}">
           <x14:formula1>
-            <xm:f>A_servicios_especialidades!$B$2:$B$100</xm:f>
+            <xm:f>E_14_GRUPOS_Programas!$A$2:$A$100</xm:f>
           </x14:formula1>
           <xm:sqref>F98:F461</xm:sqref>
         </x14:dataValidation>
@@ -693,7 +1061,7 @@
   <dimension ref="A1:H103"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -706,39 +1074,40 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B1" t="s">
-        <v>24</v>
+        <v>10</v>
       </c>
       <c r="C1" t="s">
-        <v>25</v>
+        <v>11</v>
       </c>
       <c r="D1" t="s">
-        <v>26</v>
+        <v>12</v>
       </c>
       <c r="E1" t="s">
-        <v>27</v>
+        <v>13</v>
       </c>
       <c r="F1" t="s">
-        <v>28</v>
+        <v>14</v>
       </c>
       <c r="G1" t="s">
-        <v>29</v>
+        <v>15</v>
       </c>
       <c r="H1" t="s">
-        <v>30</v>
+        <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>31</v>
+        <v>20</v>
       </c>
       <c r="B2" t="s">
-        <v>22</v>
+        <v>9</v>
       </c>
       <c r="C2" s="3">
-        <v>44621</v>
+        <f ca="1">TODAY()+1</f>
+        <v>44761</v>
       </c>
       <c r="D2" s="4">
         <v>0.41666666666666669</v>
@@ -747,8 +1116,8 @@
         <v>15</v>
       </c>
       <c r="F2" s="3">
-        <f>IF(AND(HOUR(D2)=23,HOUR(G2)=0),C2+1,C2)</f>
-        <v>44621</v>
+        <f ca="1">IF(AND(HOUR(D2)=23,HOUR(G2)=0),C2+1,C2)</f>
+        <v>44761</v>
       </c>
       <c r="G2" s="4">
         <f>D2+VALUE("00:"&amp;E2&amp;":00")</f>
@@ -1389,7 +1758,7 @@
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{7A276B75-DA65-4423-8D72-321F308D33C7}">
           <x14:formula1>
-            <xm:f>A_servicios_especialidades!$B$2:$B$27</xm:f>
+            <xm:f>E_14_GRUPOS_Programas!$A$2:$A$27</xm:f>
           </x14:formula1>
           <xm:sqref>A124:A153</xm:sqref>
         </x14:dataValidation>
@@ -1400,6 +1769,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x0101002047D94B5E73D04A80AA6844A59F543A" ma:contentTypeVersion="0" ma:contentTypeDescription="Crear nuevo documento." ma:contentTypeScope="" ma:versionID="19f8b377e75dbac3c1f2314aec064948">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="3f6edc329ff236629c56e3b879b320d0">
     <xsd:element name="properties">
@@ -1513,32 +1897,10 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8EC26224-972D-4B00-B624-0625DBEFB70E}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CA352A83-CB83-418A-87A4-DE7F5968277D}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
@@ -1553,9 +1915,16 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CA352A83-CB83-418A-87A4-DE7F5968277D}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8EC26224-972D-4B00-B624-0625DBEFB70E}">
   <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>

</xml_diff>

<commit_message>
fix plantilla configuración de calendario anual
</commit_message>
<xml_diff>
--- a/src/assets/files/15.CalendarioAnual.xlsx
+++ b/src/assets/files/15.CalendarioAnual.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\avictoria\Documents\Proyectos\AgendaDigital\ARCHIVOS PRUEBA\oficiales\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61943AF0-953C-4662-8A3F-44FA083CA7D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AEB578E1-BFC2-40BF-B8AC-5C036B717AE2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-16560" yWindow="-3274" windowWidth="16663" windowHeight="9017" activeTab="2" xr2:uid="{76E7FC68-D242-465E-8EB4-3CC40106161F}"/>
   </bookViews>
@@ -37,12 +37,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="75">
   <si>
     <t xml:space="preserve">Atención Médica Continúa </t>
-  </si>
-  <si>
-    <t>CLAVE DE UBICACIÓN</t>
   </si>
   <si>
     <t>DESCRIPCION COMPLETA DE UBICACION</t>
@@ -300,7 +297,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="47" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -308,9 +305,8 @@
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -639,310 +635,310 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" t="s">
         <v>21</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>22</v>
       </c>
-      <c r="C1" t="s">
-        <v>23</v>
-      </c>
       <c r="D1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B2" t="s">
         <v>24</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>25</v>
       </c>
-      <c r="C2" t="s">
-        <v>26</v>
-      </c>
       <c r="D2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B3" t="s">
         <v>28</v>
       </c>
-      <c r="B3" t="s">
-        <v>29</v>
-      </c>
       <c r="C3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
+        <v>29</v>
+      </c>
+      <c r="B4" t="s">
         <v>30</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" t="s">
         <v>31</v>
       </c>
-      <c r="C4" t="s">
-        <v>32</v>
-      </c>
       <c r="D4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
+        <v>32</v>
+      </c>
+      <c r="B5" t="s">
         <v>33</v>
       </c>
-      <c r="B5" t="s">
+      <c r="C5" t="s">
         <v>34</v>
       </c>
-      <c r="C5" t="s">
-        <v>35</v>
-      </c>
       <c r="D5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B6" t="s">
+        <v>35</v>
+      </c>
+      <c r="C6" t="s">
         <v>36</v>
       </c>
-      <c r="C6" t="s">
-        <v>37</v>
-      </c>
       <c r="D6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
+        <v>37</v>
+      </c>
+      <c r="B7" t="s">
         <v>38</v>
       </c>
-      <c r="B7" t="s">
+      <c r="C7" t="s">
         <v>39</v>
       </c>
-      <c r="C7" t="s">
-        <v>40</v>
-      </c>
       <c r="D7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
+        <v>40</v>
+      </c>
+      <c r="B8" t="s">
         <v>41</v>
       </c>
-      <c r="B8" t="s">
+      <c r="C8" t="s">
         <v>42</v>
       </c>
-      <c r="C8" t="s">
-        <v>43</v>
-      </c>
       <c r="D8" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B9" t="s">
+        <v>30</v>
+      </c>
+      <c r="C9" t="s">
         <v>31</v>
       </c>
-      <c r="C9" t="s">
-        <v>32</v>
-      </c>
       <c r="D9" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
+        <v>44</v>
+      </c>
+      <c r="B10" t="s">
         <v>45</v>
       </c>
-      <c r="B10" t="s">
+      <c r="C10" t="s">
         <v>46</v>
       </c>
-      <c r="C10" t="s">
-        <v>47</v>
-      </c>
       <c r="D10" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
+        <v>47</v>
+      </c>
+      <c r="B11" t="s">
         <v>48</v>
       </c>
-      <c r="B11" t="s">
+      <c r="C11" t="s">
         <v>49</v>
       </c>
-      <c r="C11" t="s">
-        <v>50</v>
-      </c>
       <c r="D11" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
+        <v>50</v>
+      </c>
+      <c r="B12" t="s">
         <v>51</v>
       </c>
-      <c r="B12" t="s">
+      <c r="C12" t="s">
         <v>52</v>
       </c>
-      <c r="C12" t="s">
-        <v>53</v>
-      </c>
       <c r="D12" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
+        <v>53</v>
+      </c>
+      <c r="B13" t="s">
         <v>54</v>
       </c>
-      <c r="B13" t="s">
+      <c r="C13" t="s">
         <v>55</v>
       </c>
-      <c r="C13" t="s">
-        <v>56</v>
-      </c>
       <c r="D13" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
+        <v>56</v>
+      </c>
+      <c r="B14" t="s">
         <v>57</v>
       </c>
-      <c r="B14" t="s">
+      <c r="C14" t="s">
         <v>58</v>
       </c>
-      <c r="C14" t="s">
-        <v>59</v>
-      </c>
       <c r="D14" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B15" t="s">
+        <v>30</v>
+      </c>
+      <c r="C15" t="s">
         <v>31</v>
       </c>
-      <c r="C15" t="s">
-        <v>32</v>
-      </c>
       <c r="D15" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B16" t="s">
+        <v>57</v>
+      </c>
+      <c r="C16" t="s">
         <v>58</v>
       </c>
-      <c r="C16" t="s">
-        <v>59</v>
-      </c>
       <c r="D16" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
+        <v>61</v>
+      </c>
+      <c r="B17" t="s">
         <v>62</v>
       </c>
-      <c r="B17" t="s">
-        <v>63</v>
-      </c>
       <c r="C17" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D17" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B18" t="s">
+        <v>57</v>
+      </c>
+      <c r="C18" t="s">
         <v>58</v>
       </c>
-      <c r="C18" t="s">
-        <v>59</v>
-      </c>
       <c r="D18" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
+        <v>64</v>
+      </c>
+      <c r="B19" t="s">
         <v>65</v>
       </c>
-      <c r="B19" t="s">
+      <c r="C19" t="s">
         <v>66</v>
       </c>
-      <c r="C19" t="s">
-        <v>67</v>
-      </c>
       <c r="D19" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
+        <v>67</v>
+      </c>
+      <c r="B20" t="s">
         <v>68</v>
       </c>
-      <c r="B20" t="s">
-        <v>69</v>
-      </c>
       <c r="C20" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D20" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
+        <v>69</v>
+      </c>
+      <c r="B21" t="s">
         <v>70</v>
       </c>
-      <c r="B21" t="s">
+      <c r="C21" t="s">
         <v>71</v>
       </c>
-      <c r="C21" t="s">
-        <v>72</v>
-      </c>
       <c r="D21" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
+        <v>72</v>
+      </c>
+      <c r="B22" t="s">
         <v>73</v>
       </c>
-      <c r="B22" t="s">
+      <c r="C22" t="s">
         <v>74</v>
       </c>
-      <c r="C22" t="s">
-        <v>75</v>
-      </c>
       <c r="D22" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.3">
@@ -973,24 +969,23 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B0BEEB7A-6427-41AA-BCE0-BEE66E749945}">
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="13.77734375" customWidth="1"/>
-    <col min="2" max="2" width="27" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="27" customWidth="1"/>
-    <col min="4" max="4" width="16.77734375" customWidth="1"/>
-    <col min="5" max="5" width="15.88671875" customWidth="1"/>
-    <col min="6" max="6" width="27" customWidth="1"/>
-    <col min="7" max="7" width="30.6640625" customWidth="1"/>
+    <col min="1" max="1" width="27" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="27" customWidth="1"/>
+    <col min="3" max="3" width="16.77734375" customWidth="1"/>
+    <col min="4" max="4" width="15.88671875" customWidth="1"/>
+    <col min="5" max="5" width="27" customWidth="1"/>
+    <col min="6" max="6" width="30.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="2" customFormat="1" ht="28.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" s="2" customFormat="1" ht="28.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>1</v>
       </c>
@@ -1009,28 +1004,22 @@
       <c r="F1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="G1" s="2" t="s">
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
         <v>7</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A2">
-        <v>6</v>
       </c>
       <c r="B2" t="s">
         <v>8</v>
       </c>
-      <c r="C2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D2" s="2" t="s">
+      <c r="C2" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E2" t="s">
+        <v>0</v>
+      </c>
+      <c r="F2" t="s">
         <v>17</v>
-      </c>
-      <c r="F2" t="s">
-        <v>0</v>
-      </c>
-      <c r="G2" t="s">
-        <v>18</v>
       </c>
     </row>
   </sheetData>
@@ -1042,13 +1031,13 @@
           <x14:formula1>
             <xm:f>E_14_GRUPOS_Programas!$A$2:$A$27</xm:f>
           </x14:formula1>
-          <xm:sqref>F29:F97</xm:sqref>
+          <xm:sqref>E29:E97</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{D7CD36EE-C343-4AF1-AFC1-30B4B1AC8850}">
           <x14:formula1>
             <xm:f>E_14_GRUPOS_Programas!$A$2:$A$100</xm:f>
           </x14:formula1>
-          <xm:sqref>F98:F461</xm:sqref>
+          <xm:sqref>E98:E461</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -1058,87 +1047,94 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D39F04C-48C3-4E87-B348-679A9F98F4DD}">
-  <dimension ref="A1:H103"/>
+  <dimension ref="A1:H100"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="18.77734375" customWidth="1"/>
-    <col min="2" max="2" width="13.88671875" customWidth="1"/>
+    <col min="1" max="1" width="18.77734375" style="5" customWidth="1"/>
+    <col min="2" max="2" width="13.88671875" style="5" customWidth="1"/>
     <col min="4" max="4" width="11.21875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.5546875" style="6"/>
     <col min="6" max="6" width="11.21875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.5546875" style="6"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+      <c r="A1" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="F1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H1" s="6" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="B1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D1" t="s">
-        <v>12</v>
-      </c>
-      <c r="E1" t="s">
-        <v>13</v>
-      </c>
-      <c r="F1" t="s">
-        <v>14</v>
-      </c>
-      <c r="G1" t="s">
-        <v>15</v>
-      </c>
-      <c r="H1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>20</v>
-      </c>
-      <c r="B2" t="s">
-        <v>9</v>
+      <c r="B2" s="5" t="s">
+        <v>8</v>
       </c>
       <c r="C2" s="3">
         <f ca="1">TODAY()+1</f>
-        <v>44761</v>
+        <v>44763</v>
       </c>
       <c r="D2" s="4">
         <v>0.41666666666666669</v>
       </c>
-      <c r="E2">
+      <c r="E2" s="6">
         <v>15</v>
       </c>
       <c r="F2" s="3">
         <f ca="1">IF(AND(HOUR(D2)=23,HOUR(G2)=0),C2+1,C2)</f>
-        <v>44761</v>
+        <v>44763</v>
       </c>
       <c r="G2" s="4">
         <f>D2+VALUE("00:"&amp;E2&amp;":00")</f>
         <v>0.42708333333333337</v>
       </c>
-      <c r="H2">
+      <c r="H2" s="6">
         <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="C3" s="5"/>
-      <c r="D3" s="5"/>
-      <c r="F3" s="5"/>
-      <c r="G3" s="5"/>
+      <c r="C3" s="3"/>
+      <c r="D3" s="4"/>
+      <c r="F3" s="3"/>
+      <c r="G3" s="4"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="B4" s="2"/>
-      <c r="C4" s="5"/>
-      <c r="D4" s="5"/>
-      <c r="F4" s="5"/>
-      <c r="G4" s="5"/>
+      <c r="C4" s="3"/>
+      <c r="D4" s="4"/>
+      <c r="F4" s="3"/>
+      <c r="G4" s="4"/>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="C5" s="3"/>
+      <c r="D5" s="4"/>
+      <c r="F5" s="3"/>
+      <c r="G5" s="4"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C6" s="3"/>
@@ -1710,46 +1706,22 @@
       <c r="F100" s="3"/>
       <c r="G100" s="4"/>
     </row>
-    <row r="101" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="C101" s="3"/>
-      <c r="D101" s="4"/>
-      <c r="F101" s="3"/>
-      <c r="G101" s="4"/>
-    </row>
-    <row r="102" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="C102" s="3"/>
-      <c r="D102" s="4"/>
-      <c r="F102" s="3"/>
-      <c r="G102" s="4"/>
-    </row>
-    <row r="103" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="C103" s="3"/>
-      <c r="D103" s="4"/>
-      <c r="F103" s="3"/>
-      <c r="G103" s="4"/>
-    </row>
   </sheetData>
-  <mergeCells count="4">
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="F3:G3"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="F4:G4"/>
-  </mergeCells>
   <dataValidations count="4">
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H5:H103" xr:uid="{77F5C645-CD51-4AFD-9FCC-469C229AAEC9}">
-      <formula1>1</formula1>
-      <formula2>100</formula2>
-    </dataValidation>
-    <dataValidation type="whole" operator="lessThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E6:E103 E2" xr:uid="{40B0490A-D9B0-4ED1-83CB-6FED982253CF}">
+    <dataValidation type="whole" operator="lessThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E97" xr:uid="{40B0490A-D9B0-4ED1-83CB-6FED982253CF}">
       <formula1>60</formula1>
     </dataValidation>
-    <dataValidation type="time" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D6:D103 D2" xr:uid="{36ED1939-987C-49F0-898A-DC4C0D21810F}">
+    <dataValidation type="time" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D97" xr:uid="{36ED1939-987C-49F0-898A-DC4C0D21810F}">
       <formula1>0</formula1>
       <formula2>0.999988425925926</formula2>
     </dataValidation>
-    <dataValidation type="date" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C6:C103 F2 F6:F103 C2" xr:uid="{6783D32D-0876-411E-BF4C-3C0E01BC8E9C}">
+    <dataValidation type="date" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F97 C2:C97" xr:uid="{6783D32D-0876-411E-BF4C-3C0E01BC8E9C}">
       <formula1>44562</formula1>
       <formula2>44926</formula2>
+    </dataValidation>
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H3:H97" xr:uid="{77F5C645-CD51-4AFD-9FCC-469C229AAEC9}">
+      <formula1>1</formula1>
+      <formula2>100</formula2>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1760,7 +1732,7 @@
           <x14:formula1>
             <xm:f>E_14_GRUPOS_Programas!$A$2:$A$27</xm:f>
           </x14:formula1>
-          <xm:sqref>A124:A153</xm:sqref>
+          <xm:sqref>A118:A147</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -1769,21 +1741,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x0101002047D94B5E73D04A80AA6844A59F543A" ma:contentTypeVersion="0" ma:contentTypeDescription="Crear nuevo documento." ma:contentTypeScope="" ma:versionID="19f8b377e75dbac3c1f2314aec064948">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="3f6edc329ff236629c56e3b879b320d0">
     <xsd:element name="properties">
@@ -1897,10 +1854,32 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CA352A83-CB83-418A-87A4-DE7F5968277D}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8EC26224-972D-4B00-B624-0625DBEFB70E}">
   <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
@@ -1915,16 +1894,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8EC26224-972D-4B00-B624-0625DBEFB70E}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CA352A83-CB83-418A-87A4-DE7F5968277D}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>

</xml_diff>

<commit_message>
Revert "Merge branch 'EduardoP' of https://github.com/aealcantar/gui-mst-adt-web into EduardoP"
This reverts commit 645ba0aefa34010e1a5a7c049e2d8cffff0e7f96, reversing
changes made to 0265b1edc60fff712bc1e089da03762fe6abf408.
</commit_message>
<xml_diff>
--- a/src/assets/files/15.CalendarioAnual.xlsx
+++ b/src/assets/files/15.CalendarioAnual.xlsx
@@ -1,19 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\avictoria\Documents\Proyectos\AgendaDigital\ARCHIVOS PRUEBA\oficiales\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61943AF0-953C-4662-8A3F-44FA083CA7D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{75B177DF-0262-482C-9876-D06D811FD845}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-16560" yWindow="-3274" windowWidth="16663" windowHeight="9017" activeTab="2" xr2:uid="{76E7FC68-D242-465E-8EB4-3CC40106161F}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" activeTab="2" xr2:uid="{76E7FC68-D242-465E-8EB4-3CC40106161F}"/>
   </bookViews>
   <sheets>
-    <sheet name="E_14_GRUPOS_Programas" sheetId="1" r:id="rId1"/>
+    <sheet name="A_servicios_especialidades" sheetId="1" r:id="rId1"/>
     <sheet name="B_4_UBICACIONES" sheetId="2" r:id="rId2"/>
     <sheet name="F_CalendarioAnual" sheetId="3" r:id="rId3"/>
   </sheets>
@@ -37,7 +37,46 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="34">
+  <si>
+    <t>CLAVE ESPECIALIDAD</t>
+  </si>
+  <si>
+    <t>DESCRIPCIÓN ESPECIALIDAD</t>
+  </si>
+  <si>
+    <t>IND_CE</t>
+  </si>
+  <si>
+    <t>IND_HOSP</t>
+  </si>
+  <si>
+    <t>IND_IQ</t>
+  </si>
+  <si>
+    <t>IND_NIVEL1</t>
+  </si>
+  <si>
+    <t>IND_NIVEL2</t>
+  </si>
+  <si>
+    <t>IND_NIVEL3</t>
+  </si>
+  <si>
+    <t>IND_CSS</t>
+  </si>
+  <si>
+    <t>FEC_BAJA</t>
+  </si>
+  <si>
+    <t>FEC_ALTA</t>
+  </si>
+  <si>
+    <t>FEC_ACTUALIZACION</t>
+  </si>
+  <si>
+    <t>AC01</t>
+  </si>
   <si>
     <t xml:space="preserve">Atención Médica Continúa </t>
   </si>
@@ -69,6 +108,9 @@
     <t>Trab_Social_01</t>
   </si>
   <si>
+    <t>SERVICIOS / ESPECIALIDADES</t>
+  </si>
+  <si>
     <t>UBICACIÓN</t>
   </si>
   <si>
@@ -90,181 +132,13 @@
     <t>MAXIMO DE PARTICIPANTES</t>
   </si>
   <si>
+    <t>Adulto Mayores</t>
+  </si>
+  <si>
     <t>Consultorio</t>
   </si>
   <si>
     <t>UMF12</t>
-  </si>
-  <si>
-    <t>PROGRAMA</t>
-  </si>
-  <si>
-    <t>VIH</t>
-  </si>
-  <si>
-    <t>DESCRIPCION GRUPO / PROGRAMA</t>
-  </si>
-  <si>
-    <t>CODIGO</t>
-  </si>
-  <si>
-    <t>DESCRIPCION ACTIVIDAD</t>
-  </si>
-  <si>
-    <t>Tour  Quirúrgico</t>
-  </si>
-  <si>
-    <t>TS2.C</t>
-  </si>
-  <si>
-    <t>Tour Quirúrgico</t>
-  </si>
-  <si>
-    <t>Trabajo Social</t>
-  </si>
-  <si>
-    <t>Tour Obstétrico</t>
-  </si>
-  <si>
-    <t>TS2.B</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Tour Quimioterapia</t>
-  </si>
-  <si>
-    <t>Z71.8</t>
-  </si>
-  <si>
-    <t>Necesidad de información sobre cáncer</t>
-  </si>
-  <si>
-    <t>Donación de  Sangre.</t>
-  </si>
-  <si>
-    <t>TS1.O</t>
-  </si>
-  <si>
-    <t>Necesidad de información para donación de sangre</t>
-  </si>
-  <si>
-    <t>TS1.T</t>
-  </si>
-  <si>
-    <t>Paciente integrado a programa de VIH/SIDA</t>
-  </si>
-  <si>
-    <t>Diálisis</t>
-  </si>
-  <si>
-    <t>TS1.W</t>
-  </si>
-  <si>
-    <t>Paciente integrado a programa de Diálisis</t>
-  </si>
-  <si>
-    <t>Hemodiálisis</t>
-  </si>
-  <si>
-    <t>TS1.U</t>
-  </si>
-  <si>
-    <t>Paciente integrado a programa de Hemodiálisis</t>
-  </si>
-  <si>
-    <t>CACU</t>
-  </si>
-  <si>
-    <t>CAMA</t>
-  </si>
-  <si>
-    <t>TS1.X</t>
-  </si>
-  <si>
-    <t>Paciente integrado a clínica de mama</t>
-  </si>
-  <si>
-    <t>GeriatrIMSS</t>
-  </si>
-  <si>
-    <t>TS1</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> </t>
-  </si>
-  <si>
-    <t>Lactancia Materna</t>
-  </si>
-  <si>
-    <t>TS1.S</t>
-  </si>
-  <si>
-    <t>Necesidad de información para la lactancia materna</t>
-  </si>
-  <si>
-    <t>Cuidados del paciente post trasplante</t>
-  </si>
-  <si>
-    <t>TS1.N</t>
-  </si>
-  <si>
-    <t>Necesidad de información para donación de órganos y tejidos</t>
-  </si>
-  <si>
-    <t>Educación para pacientes prematuros</t>
-  </si>
-  <si>
-    <t>TS1.L</t>
-  </si>
-  <si>
-    <t>Expectativas diferentes de los integrantes de la familia que inciden en salud</t>
-  </si>
-  <si>
-    <t>Cuidados de pacientes oncológicos</t>
-  </si>
-  <si>
-    <t>Autocuidado de la Salud</t>
-  </si>
-  <si>
-    <t>Cuidados post cateterismo cardiaco</t>
-  </si>
-  <si>
-    <t>Ts2</t>
-  </si>
-  <si>
-    <t>Yoga prenatal</t>
-  </si>
-  <si>
-    <t>Grupos voluntarios</t>
-  </si>
-  <si>
-    <t>TS2.H</t>
-  </si>
-  <si>
-    <t>Incorporación a grupos de autoayuda</t>
-  </si>
-  <si>
-    <t>Otros</t>
-  </si>
-  <si>
-    <t>TS3</t>
-  </si>
-  <si>
-    <t>ADEC</t>
-  </si>
-  <si>
-    <t>TS1.V</t>
-  </si>
-  <si>
-    <t>Paciente integrado al programa de DEC</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Planificación Familiar </t>
-  </si>
-  <si>
-    <t>Z30.0</t>
-  </si>
-  <si>
-    <t>Necesidad de información en Planificación Familiar</t>
   </si>
 </sst>
 </file>
@@ -625,346 +499,104 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{64CCAEAA-4231-4770-9010-191EE5FD3295}">
-  <dimension ref="A1:J191"/>
+  <dimension ref="A1:L191"/>
   <sheetViews>
     <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="I17" sqref="I17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="23.33203125" customWidth="1"/>
-    <col min="4" max="4" width="21.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>21</v>
+        <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>22</v>
+        <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>23</v>
+        <v>2</v>
       </c>
       <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="B2" t="s">
-        <v>25</v>
-      </c>
-      <c r="C2" t="s">
-        <v>26</v>
-      </c>
-      <c r="D2" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>28</v>
-      </c>
-      <c r="B3" t="s">
-        <v>29</v>
-      </c>
-      <c r="C3" t="s">
-        <v>28</v>
-      </c>
-      <c r="D3" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>30</v>
-      </c>
-      <c r="B4" t="s">
-        <v>31</v>
-      </c>
-      <c r="C4" t="s">
-        <v>32</v>
-      </c>
-      <c r="D4" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>33</v>
-      </c>
-      <c r="B5" t="s">
-        <v>34</v>
-      </c>
-      <c r="C5" t="s">
-        <v>35</v>
-      </c>
-      <c r="D5" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>20</v>
-      </c>
-      <c r="B6" t="s">
-        <v>36</v>
-      </c>
-      <c r="C6" t="s">
-        <v>37</v>
-      </c>
-      <c r="D6" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>38</v>
-      </c>
-      <c r="B7" t="s">
-        <v>39</v>
-      </c>
-      <c r="C7" t="s">
-        <v>40</v>
-      </c>
-      <c r="D7" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>41</v>
-      </c>
-      <c r="B8" t="s">
-        <v>42</v>
-      </c>
-      <c r="C8" t="s">
-        <v>43</v>
-      </c>
-      <c r="D8" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
-        <v>44</v>
-      </c>
-      <c r="B9" t="s">
-        <v>31</v>
-      </c>
-      <c r="C9" t="s">
-        <v>32</v>
-      </c>
-      <c r="D9" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
-        <v>45</v>
-      </c>
-      <c r="B10" t="s">
-        <v>46</v>
-      </c>
-      <c r="C10" t="s">
-        <v>47</v>
-      </c>
-      <c r="D10" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
-        <v>48</v>
-      </c>
-      <c r="B11" t="s">
-        <v>49</v>
-      </c>
-      <c r="C11" t="s">
-        <v>50</v>
-      </c>
-      <c r="D11" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
-        <v>51</v>
-      </c>
-      <c r="B12" t="s">
-        <v>52</v>
-      </c>
-      <c r="C12" t="s">
-        <v>53</v>
-      </c>
-      <c r="D12" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
-        <v>54</v>
-      </c>
-      <c r="B13" t="s">
-        <v>55</v>
-      </c>
-      <c r="C13" t="s">
-        <v>56</v>
-      </c>
-      <c r="D13" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
-        <v>57</v>
-      </c>
-      <c r="B14" t="s">
-        <v>58</v>
-      </c>
-      <c r="C14" t="s">
-        <v>59</v>
-      </c>
-      <c r="D14" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
-        <v>60</v>
-      </c>
-      <c r="B15" t="s">
-        <v>31</v>
-      </c>
-      <c r="C15" t="s">
-        <v>32</v>
-      </c>
-      <c r="D15" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
-        <v>61</v>
-      </c>
-      <c r="B16" t="s">
-        <v>58</v>
-      </c>
-      <c r="C16" t="s">
-        <v>59</v>
-      </c>
-      <c r="D16" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
-        <v>62</v>
-      </c>
-      <c r="B17" t="s">
-        <v>63</v>
-      </c>
-      <c r="C17" t="s">
-        <v>50</v>
-      </c>
-      <c r="D17" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
-        <v>64</v>
-      </c>
-      <c r="B18" t="s">
-        <v>58</v>
-      </c>
-      <c r="C18" t="s">
-        <v>59</v>
-      </c>
-      <c r="D18" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A19" t="s">
-        <v>65</v>
-      </c>
-      <c r="B19" t="s">
-        <v>66</v>
-      </c>
-      <c r="C19" t="s">
-        <v>67</v>
-      </c>
-      <c r="D19" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A20" t="s">
-        <v>68</v>
-      </c>
-      <c r="B20" t="s">
-        <v>69</v>
-      </c>
-      <c r="C20" t="s">
-        <v>50</v>
-      </c>
-      <c r="D20" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A21" t="s">
-        <v>70</v>
-      </c>
-      <c r="B21" t="s">
-        <v>71</v>
-      </c>
-      <c r="C21" t="s">
-        <v>72</v>
-      </c>
-      <c r="D21" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A22" t="s">
-        <v>73</v>
-      </c>
-      <c r="B22" t="s">
-        <v>74</v>
-      </c>
-      <c r="C22" t="s">
-        <v>75</v>
-      </c>
-      <c r="D22" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="I26" s="1"/>
-    </row>
-    <row r="42" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I42" s="1"/>
-    </row>
-    <row r="43" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I43" s="1"/>
-    </row>
-    <row r="52" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I52" s="1"/>
-    </row>
-    <row r="65" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I65" s="1"/>
-    </row>
-    <row r="190" spans="10:10" x14ac:dyDescent="0.3">
-      <c r="J190" s="1"/>
-    </row>
-    <row r="191" spans="10:10" x14ac:dyDescent="0.3">
-      <c r="J191" s="1"/>
+        <v>13</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="E2">
+        <v>0</v>
+      </c>
+      <c r="F2">
+        <v>1</v>
+      </c>
+      <c r="G2">
+        <v>1</v>
+      </c>
+      <c r="H2">
+        <v>1</v>
+      </c>
+      <c r="I2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="10:10" x14ac:dyDescent="0.3">
+      <c r="J26" s="1"/>
+    </row>
+    <row r="42" spans="10:10" x14ac:dyDescent="0.3">
+      <c r="J42" s="1"/>
+    </row>
+    <row r="43" spans="10:10" x14ac:dyDescent="0.3">
+      <c r="J43" s="1"/>
+    </row>
+    <row r="52" spans="10:10" x14ac:dyDescent="0.3">
+      <c r="J52" s="1"/>
+    </row>
+    <row r="65" spans="10:10" x14ac:dyDescent="0.3">
+      <c r="J65" s="1"/>
+    </row>
+    <row r="190" spans="11:11" x14ac:dyDescent="0.3">
+      <c r="K190" s="1"/>
+    </row>
+    <row r="191" spans="11:11" x14ac:dyDescent="0.3">
+      <c r="K191" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -992,25 +624,25 @@
   <sheetData>
     <row r="1" spans="1:7" s="2" customFormat="1" ht="28.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>2</v>
+        <v>15</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>3</v>
+        <v>16</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>4</v>
+        <v>17</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>5</v>
+        <v>18</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>6</v>
+        <v>19</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>7</v>
+        <v>20</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
@@ -1018,19 +650,19 @@
         <v>6</v>
       </c>
       <c r="B2" t="s">
-        <v>8</v>
+        <v>21</v>
       </c>
       <c r="C2" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>17</v>
+        <v>32</v>
       </c>
       <c r="F2" t="s">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="G2" t="s">
-        <v>18</v>
+        <v>33</v>
       </c>
     </row>
   </sheetData>
@@ -1040,13 +672,13 @@
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{5262BBD6-F35A-4EFA-8784-122DD4E3CC3F}">
           <x14:formula1>
-            <xm:f>E_14_GRUPOS_Programas!$A$2:$A$27</xm:f>
+            <xm:f>A_servicios_especialidades!$B$2:$B$27</xm:f>
           </x14:formula1>
           <xm:sqref>F29:F97</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{D7CD36EE-C343-4AF1-AFC1-30B4B1AC8850}">
           <x14:formula1>
-            <xm:f>E_14_GRUPOS_Programas!$A$2:$A$100</xm:f>
+            <xm:f>A_servicios_especialidades!$B$2:$B$100</xm:f>
           </x14:formula1>
           <xm:sqref>F98:F461</xm:sqref>
         </x14:dataValidation>
@@ -1061,7 +693,7 @@
   <dimension ref="A1:H103"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1074,40 +706,39 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="B1" t="s">
-        <v>10</v>
+        <v>24</v>
       </c>
       <c r="C1" t="s">
-        <v>11</v>
+        <v>25</v>
       </c>
       <c r="D1" t="s">
-        <v>12</v>
+        <v>26</v>
       </c>
       <c r="E1" t="s">
-        <v>13</v>
+        <v>27</v>
       </c>
       <c r="F1" t="s">
-        <v>14</v>
+        <v>28</v>
       </c>
       <c r="G1" t="s">
-        <v>15</v>
+        <v>29</v>
       </c>
       <c r="H1" t="s">
-        <v>16</v>
+        <v>30</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>20</v>
+        <v>31</v>
       </c>
       <c r="B2" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="C2" s="3">
-        <f ca="1">TODAY()+1</f>
-        <v>44761</v>
+        <v>44621</v>
       </c>
       <c r="D2" s="4">
         <v>0.41666666666666669</v>
@@ -1116,8 +747,8 @@
         <v>15</v>
       </c>
       <c r="F2" s="3">
-        <f ca="1">IF(AND(HOUR(D2)=23,HOUR(G2)=0),C2+1,C2)</f>
-        <v>44761</v>
+        <f>IF(AND(HOUR(D2)=23,HOUR(G2)=0),C2+1,C2)</f>
+        <v>44621</v>
       </c>
       <c r="G2" s="4">
         <f>D2+VALUE("00:"&amp;E2&amp;":00")</f>
@@ -1758,7 +1389,7 @@
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{7A276B75-DA65-4423-8D72-321F308D33C7}">
           <x14:formula1>
-            <xm:f>E_14_GRUPOS_Programas!$A$2:$A$27</xm:f>
+            <xm:f>A_servicios_especialidades!$B$2:$B$27</xm:f>
           </x14:formula1>
           <xm:sqref>A124:A153</xm:sqref>
         </x14:dataValidation>
@@ -1769,21 +1400,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x0101002047D94B5E73D04A80AA6844A59F543A" ma:contentTypeVersion="0" ma:contentTypeDescription="Crear nuevo documento." ma:contentTypeScope="" ma:versionID="19f8b377e75dbac3c1f2314aec064948">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="3f6edc329ff236629c56e3b879b320d0">
     <xsd:element name="properties">
@@ -1897,10 +1513,32 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CA352A83-CB83-418A-87A4-DE7F5968277D}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8EC26224-972D-4B00-B624-0625DBEFB70E}">
   <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
@@ -1915,16 +1553,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8EC26224-972D-4B00-B624-0625DBEFB70E}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CA352A83-CB83-418A-87A4-DE7F5968277D}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>

</xml_diff>